<commit_message>
enviando o projeto 5
</commit_message>
<xml_diff>
--- a/Projeto 2/intel.xlsx
+++ b/Projeto 2/intel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1765,7 +1765,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>